<commit_message>
Correcciones y modificaciones en sprint backlog 1, aun queda pendiente sprint backlog 2
</commit_message>
<xml_diff>
--- a/Documentos/PETAPP_SPRINTBL.xlsx
+++ b/Documentos/PETAPP_SPRINTBL.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Task</t>
   </si>
@@ -66,7 +66,13 @@
     <t>Sprint Backlog 1</t>
   </si>
   <si>
-    <t>Autor: Luis Gianpierre Portella Bravo</t>
+    <t>Autores:</t>
+  </si>
+  <si>
+    <t>Luis Gianpierre Portella Bravo</t>
+  </si>
+  <si>
+    <t>Hans Soto Rojas</t>
   </si>
 </sst>
 </file>
@@ -202,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -229,12 +235,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -530,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I22"/>
+  <dimension ref="A2:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,12 +632,24 @@
       <c r="C6" s="8">
         <v>8</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
+      <c r="D6" s="8">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="10"/>
@@ -612,12 +659,24 @@
       <c r="C7" s="8">
         <v>8</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
+      <c r="D7" s="8">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8">
+        <v>8</v>
+      </c>
+      <c r="F7" s="8">
+        <v>6</v>
+      </c>
+      <c r="G7" s="8">
+        <v>4</v>
+      </c>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
@@ -642,7 +701,9 @@
       <c r="H8" s="8">
         <v>0</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
@@ -652,12 +713,24 @@
       <c r="C9" s="8">
         <v>8</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="D9" s="8">
+        <v>8</v>
+      </c>
+      <c r="E9" s="8">
+        <v>7</v>
+      </c>
+      <c r="F9" s="8">
+        <v>3</v>
+      </c>
+      <c r="G9" s="8">
+        <v>3</v>
+      </c>
+      <c r="H9" s="8">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
@@ -682,7 +755,9 @@
       <c r="H10" s="8">
         <v>8</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
@@ -710,8 +785,18 @@
       <c r="A13" s="1"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="12" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>